<commit_message>
working on fixing def recognize()
</commit_message>
<xml_diff>
--- a/Selector Summary.xlsx
+++ b/Selector Summary.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -93,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,6 +116,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -181,7 +184,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -197,7 +200,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,7 +228,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O22" activeCellId="0" sqref="O22"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1191,4 +1194,30 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>